<commit_message>
unittest_case is error after exit
</commit_message>
<xml_diff>
--- a/interfaceTest/testFile/userCase.xlsx
+++ b/interfaceTest/testFile/userCase.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>case_name</t>
   </si>
@@ -29,6 +29,18 @@
   </si>
   <si>
     <t>login</t>
+  </si>
+  <si>
+    <t>https://api.app.aixiangdao.tech/develop/mms/user/login</t>
+  </si>
+  <si>
+    <t>"userName": "15721484677", "password": "484677"</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>college</t>
   </si>
   <si>
     <t>http://zuowen.api.juhe.cn/zuowen/typeList</t>
@@ -50,13 +62,19 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.3"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="9.75"/>
@@ -65,6 +83,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -119,6 +144,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -160,6 +192,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -167,21 +206,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -190,20 +222,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,18 +236,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -242,163 +302,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -530,10 +548,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -542,142 +560,146 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1026,13 +1048,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="18.625" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
@@ -1040,7 +1062,7 @@
     <col min="4" max="4" width="13.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" spans="1:4">
+    <row r="1" ht="14.25" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1053,60 +1075,71 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1"/>
     </row>
-    <row r="2" ht="14.25" spans="1:4">
-      <c r="A2" s="1" t="s">
+    <row r="2" ht="30" customHeight="1" spans="1:5">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+    <row r="3" ht="14.25" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://zuowen.api.juhe.cn/zuowen/typeList" tooltip="http://zuowen.api.juhe.cn/zuowen/typeList"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://api.app.aixiangdao.tech/develop/mms/user/login" tooltip="https://api.app.aixiangdao.tech/develop/mms/user/login"/>
+    <hyperlink ref="B3" r:id="rId2" display="http://zuowen.api.juhe.cn/zuowen/typeList" tooltip="http://zuowen.api.juhe.cn/zuowen/typeList"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
fix json type is int info
</commit_message>
<xml_diff>
--- a/interfaceTest/testFile/userCase.xlsx
+++ b/interfaceTest/testFile/userCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12465" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12465"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>method</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>"优惠券列表"</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>https://api.aixiangdao.com/message/app/message/countUnRead</t>
+  </si>
+  <si>
+    <t>"写入"</t>
   </si>
 </sst>
 </file>
@@ -682,7 +691,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -691,6 +700,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1048,8 +1058,8 @@
   <sheetPr/>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1064,186 +1074,186 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1258,17 +1268,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="11.25" customWidth="1"/>
     <col min="2" max="2" width="72.5" customWidth="1"/>
-    <col min="3" max="3" width="35.5" customWidth="1"/>
+    <col min="3" max="3" width="39.125" customWidth="1"/>
     <col min="4" max="4" width="45" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1309,6 +1319,17 @@
       </c>
       <c r="D3" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add code error is send logs
</commit_message>
<xml_diff>
--- a/interfaceTest/testFile/userCase.xlsx
+++ b/interfaceTest/testFile/userCase.xlsx
@@ -97,8 +97,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -128,9 +128,106 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -150,103 +247,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -264,6 +264,138 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -289,138 +421,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -455,45 +455,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -508,26 +469,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -555,16 +496,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -573,16 +573,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -594,112 +594,112 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1269,7 +1269,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
rewrite response check code
</commit_message>
<xml_diff>
--- a/interfaceTest/testFile/userCase.xlsx
+++ b/interfaceTest/testFile/userCase.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView windowWidth="28800" windowHeight="12540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="Interface" sheetId="2" r:id="rId2"/>
+    <sheet name="Response" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>method</t>
   </si>
@@ -47,7 +48,7 @@
     <t>post</t>
   </si>
   <si>
-    <t>https://m.api.aixiangdao.com/user/app/user/info</t>
+    <t>https://m.api.aixiangdao.tech/P20190825/user/app/user/info</t>
   </si>
   <si>
     <t>{"clientType":"miniApp"}</t>
@@ -59,7 +60,7 @@
     <t>Mozilla/5.0 (iPhone; CPU iPhone OS 10_3_3 like Mac OS X) AppleWebKit/603.3.8 (KHTML, like Gecko) Mobile/14G60 MicroMessenger/7.0.2(0x17000222) NetType/WIFI Language/zh_CN</t>
   </si>
   <si>
-    <t>03-01512000578944964338-88000327-1570859531</t>
+    <t>03-01623036633318875191-71902003-1571644344</t>
   </si>
   <si>
     <t>"登陆"</t>
@@ -71,13 +72,22 @@
     <t>Interface</t>
   </si>
   <si>
-    <t>https://m.api.aixiangdao.com/order/app/getOrders</t>
-  </si>
-  <si>
-    <t>{"pageIndex":0,"pageSize":10,"orderType":2,"clientType":"miniApp"}</t>
-  </si>
-  <si>
-    <t>"商品订单页"</t>
+    <t>https://m.api.aixiangdao.tech/P20190825/basic/app/location/city</t>
+  </si>
+  <si>
+    <t>{"latitude":31.29686,"longitude":121.4576,"clientType":"miniApp"}</t>
+  </si>
+  <si>
+    <t>"城市"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chech_Response </t>
+  </si>
+  <si>
+    <t>cashCouponTotalCount</t>
+  </si>
+  <si>
+    <t>result</t>
   </si>
 </sst>
 </file>
@@ -691,8 +701,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1056,8 +1069,8 @@
   <sheetPr/>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1074,57 +1087,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="I2" t="s">
@@ -1132,118 +1145,118 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://m.api.aixiangdao.com/user/app/user/info" tooltip="https://m.api.aixiangdao.com/user/app/user/info"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://m.api.aixiangdao.tech/P20190825/user/app/user/info" tooltip="https://m.api.aixiangdao.tech/P20190825/user/app/user/info"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1256,8 +1269,8 @@
   <sheetPr/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="3"/>
@@ -1283,10 +1296,10 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
@@ -1297,26 +1310,87 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://m.api.aixiangdao.com/order/app/getOrders" tooltip="https://m.api.aixiangdao.com/order/app/getOrders"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://m.api.aixiangdao.tech/P20190825/basic/app/location/city" tooltip="https://m.api.aixiangdao.tech/P20190825/basic/app/location/city"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="2" max="2" width="22.25" customWidth="1"/>
+    <col min="3" max="3" width="10.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="17" customHeight="1" spans="1:24">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:X1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>